<commit_message>
removed unrelated sheets from SRA accession list
</commit_message>
<xml_diff>
--- a/SRA_Accession_list.xlsx
+++ b/SRA_Accession_list.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11360" yWindow="1660" windowWidth="19160" windowHeight="10520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14080" yWindow="4160" windowWidth="18520" windowHeight="10520" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,103 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="107">
-  <si>
-    <t>chickpeas</t>
-  </si>
-  <si>
-    <t>black beans</t>
-  </si>
-  <si>
-    <t>kidney beans</t>
-  </si>
-  <si>
-    <t>edamame</t>
-  </si>
-  <si>
-    <t>Protein</t>
-  </si>
-  <si>
-    <t>protein powder</t>
-  </si>
-  <si>
-    <t>tru-nut powder</t>
-  </si>
-  <si>
-    <t>brown rice</t>
-  </si>
-  <si>
-    <t>white rice</t>
-  </si>
-  <si>
-    <t>quinoa</t>
-  </si>
-  <si>
-    <t>oats</t>
-  </si>
-  <si>
-    <t>ezekiel bread</t>
-  </si>
-  <si>
-    <t>red lentils</t>
-  </si>
-  <si>
-    <t>brown lentils</t>
-  </si>
-  <si>
-    <t>wheat flour</t>
-  </si>
-  <si>
-    <t>ripe banana</t>
-  </si>
-  <si>
-    <t>unripe banana</t>
-  </si>
-  <si>
-    <t>blackberry</t>
-  </si>
-  <si>
-    <t>raspberry</t>
-  </si>
-  <si>
-    <t>blueberry</t>
-  </si>
-  <si>
-    <t>strawberry</t>
-  </si>
-  <si>
-    <t>mango</t>
-  </si>
-  <si>
-    <t>orange</t>
-  </si>
-  <si>
-    <t>apple</t>
-  </si>
-  <si>
-    <t>canteloupe</t>
-  </si>
-  <si>
-    <t>grapes</t>
-  </si>
-  <si>
-    <t>spinach</t>
-  </si>
-  <si>
-    <t>carrots</t>
-  </si>
-  <si>
-    <t>tomatoes</t>
-  </si>
-  <si>
-    <t>lettuce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brocoli </t>
-  </si>
-  <si>
-    <t>red cabbage</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="75">
   <si>
     <t>Hagfish (Myxini)</t>
   </si>
@@ -696,400 +599,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:A38"/>
-  <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I3">
         <v>4000</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I4">
         <v>20000</v>
       </c>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="K4" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I5">
         <v>5000</v>
       </c>
       <c r="J5" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="K5" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I6">
         <v>9000</v>
       </c>
       <c r="J6" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1097,232 +822,232 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
         <v>57</v>
       </c>
-      <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" t="s">
-        <v>89</v>
-      </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="I8" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="K8" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="K9" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J10" t="s">
-        <v>86</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
         <v>57</v>
       </c>
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" t="s">
-        <v>89</v>
-      </c>
       <c r="G11" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="G13" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="I13" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="K13" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="H16" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I16" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="J16" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="K16" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1345,7 +1070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B5"/>
   <sheetViews>
@@ -1357,25 +1082,25 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>